<commit_message>
add color code and reference paper
</commit_message>
<xml_diff>
--- a/potential_comparisons.xlsx
+++ b/potential_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\FFparamOpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A89E4D3-E8BC-42F1-8561-2A02996C1BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985A5D44-4C64-45E6-86C7-420E056222DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F2428AE-CAB2-46BB-89A9-AC6BC53BC595}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Model name</t>
   </si>
@@ -90,16 +90,25 @@
     <t>Simulated structure of?</t>
   </si>
   <si>
-    <t>pure silica</t>
-  </si>
-  <si>
-    <t>sodium silicate</t>
-  </si>
-  <si>
-    <t>soda-lime glass</t>
-  </si>
-  <si>
     <t>Results of sims</t>
+  </si>
+  <si>
+    <t>sodium borosilicate</t>
+  </si>
+  <si>
+    <t>pure silica: Soules [3–5]</t>
+  </si>
+  <si>
+    <t>sodium-potassium</t>
+  </si>
+  <si>
+    <t>aluminosilicate glasses</t>
+  </si>
+  <si>
+    <t>soda-lime glass: Garofalini et al. [8,9]</t>
+  </si>
+  <si>
+    <t>Use different shades of blue to distinguish between author's in that following model</t>
   </si>
 </sst>
 </file>
@@ -115,15 +124,27 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,20 +152,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,45 +587,47 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7BC2C4-3346-496E-87E6-5BB512E30292}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
-        <v>13</v>
+      <c r="G1" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -592,43 +637,66 @@
       <c r="C2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>10</v>
+      <c r="F2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="D2:D6"/>
+    <mergeCell ref="C2:C6"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="E2:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add more potential and TBDs
</commit_message>
<xml_diff>
--- a/potential_comparisons.xlsx
+++ b/potential_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\School\FFparamOpt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B979D04-7B95-4F18-8108-5F2837DEDC41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386676A5-C8E5-4D08-AA71-98A1A833B5D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4F2428AE-CAB2-46BB-89A9-AC6BC53BC595}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="1">
+  <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -48,17 +48,37 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="1">
+  <valueMetadata count="3">
     <bk>
       <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Model name</t>
   </si>
@@ -133,6 +153,45 @@
   </si>
   <si>
     <t>vitreous glass: Garofalini et al. [8,9]</t>
+  </si>
+  <si>
+    <t>Partial charge</t>
+  </si>
+  <si>
+    <t>TTAM Tsuneyuki et al.[4]</t>
+  </si>
+  <si>
+    <t>N-Body</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Pedone Potential (PMMCS)</t>
+  </si>
+  <si>
+    <t>https://sites.google.com/site/compmaterchem/downloads</t>
+  </si>
+  <si>
+    <t>repulsion between electron charge clouds (short)</t>
+  </si>
+  <si>
+    <t>Composed of?</t>
+  </si>
+  <si>
+    <t>Buckingham potential</t>
+  </si>
+  <si>
+    <t>Coulomb pair potential</t>
+  </si>
+  <si>
+    <t>Morse potential</t>
+  </si>
+  <si>
+    <t>Repulsive contribution (Bij/r): prevent collapse at high temp</t>
   </si>
 </sst>
 </file>
@@ -260,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -269,47 +328,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -369,9 +440,17 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <rv s="0">
     <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -389,6 +468,8 @@
 <file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -709,28 +790,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF7BC2C4-3346-496E-87E6-5BB512E30292}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.21875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="19" customWidth="1"/>
+    <col min="2" max="2" width="18" style="19" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="20" customWidth="1"/>
+    <col min="6" max="6" width="23.109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="17.21875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -739,146 +822,283 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="6" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:13" s="4" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7" t="e" vm="1">
+      <c r="C2" s="11" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="9">
+        <v>2</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="I2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="16"/>
-      <c r="K3" t="s">
+    <row r="3" spans="1:13" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="8"/>
+      <c r="M3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="13" t="s">
+    <row r="4" spans="1:13" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="3" t="s">
+    <row r="6" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="3" t="s">
+    <row r="7" spans="1:13" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="3" t="s">
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="17" t="s">
+    <row r="9" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="17" t="s">
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="I10" s="10"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="11" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="11" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="12"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="G9:G10"/>
+  <mergeCells count="25">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="E13:E15"/>
+    <mergeCell ref="G13:G15"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="A2:A10"/>
     <mergeCell ref="B2:B10"/>
     <mergeCell ref="C2:C10"/>
     <mergeCell ref="D2:D10"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="H4:H5"/>
     <mergeCell ref="E2:E10"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="F2:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added functional form for TTAM and Pedone Potential
</commit_message>
<xml_diff>
--- a/potential_comparisons.xlsx
+++ b/potential_comparisons.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresramos/Desktop/Projectarbeit/FFparamOpt/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C418EA9C-C5A5-1B4F-9751-1472D6BC728B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0A0BB5-11D0-9A41-80A5-5FBD8D032CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="26880" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Model name</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Rigid ionic model</t>
-  </si>
-  <si>
-    <t>#VALUE!</t>
   </si>
   <si>
     <t>https://docs.lammps.org/pair_buck.html</t>
@@ -463,6 +460,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -474,60 +525,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -552,9 +549,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
+      <xdr:colOff>374650</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
+      <xdr:rowOff>342900</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4438650" cy="749300"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -572,7 +569,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4933950" y="800100"/>
+              <a:off x="4832350" y="952500"/>
               <a:ext cx="4438650" cy="749300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1030,7 +1027,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4933950" y="800100"/>
+              <a:off x="4832350" y="952500"/>
               <a:ext cx="4438650" cy="749300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1181,6 +1178,1069 @@
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
                 <a:t>𝑖𝑗 )</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1800"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>781050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2952750" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D041EAFE-0A6B-0B4E-8463-7726C3B52F1D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5238750" y="4013200"/>
+              <a:ext cx="2952750" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1800" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑞</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑞</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑒</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐴</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖𝑗</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑒</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>/</m:t>
+                        </m:r>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝜌</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐶</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑟</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>6</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1800"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D041EAFE-0A6B-0B4E-8463-7726C3B52F1D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5238750" y="4013200"/>
+              <a:ext cx="2952750" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑞</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑞</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑒</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟+𝐴_𝑖𝑗 𝑒^(−𝑟/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜌_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖𝑗 )−𝐶_𝑖𝑗/𝑟^6 </a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1800"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>298450</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4591050" cy="749300"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA944D43-B7D7-C647-9E99-CF016FFF9D81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4756150" y="6337300"/>
+              <a:ext cx="4591050" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="left"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1800" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑞</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑞</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="en-US" sz="1800" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑒</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>2</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>+</m:t>
+                    </m:r>
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝐷</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑖𝑗</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>[</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:d>
+                          <m:dPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:dPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>1−</m:t>
+                            </m:r>
+                            <m:sSup>
+                              <m:sSupPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSupPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑒</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sup>
+                                <m:r>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>−</m:t>
+                                </m:r>
+                                <m:sSub>
+                                  <m:sSubPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:sSubPr>
+                                  <m:e>
+                                    <m:r>
+                                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑎</m:t>
+                                    </m:r>
+                                  </m:e>
+                                  <m:sub>
+                                    <m:r>
+                                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>𝑖𝑗</m:t>
+                                    </m:r>
+                                  </m:sub>
+                                </m:sSub>
+                                <m:d>
+                                  <m:dPr>
+                                    <m:ctrlPr>
+                                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                    </m:ctrlPr>
+                                  </m:dPr>
+                                  <m:e>
+                                    <m:sSub>
+                                      <m:sSubPr>
+                                        <m:ctrlPr>
+                                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                        </m:ctrlPr>
+                                      </m:sSubPr>
+                                      <m:e>
+                                        <m:r>
+                                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>𝑟</m:t>
+                                        </m:r>
+                                      </m:e>
+                                      <m:sub>
+                                        <m:r>
+                                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>𝑖𝑗</m:t>
+                                        </m:r>
+                                      </m:sub>
+                                    </m:sSub>
+                                    <m:r>
+                                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                      </a:rPr>
+                                      <m:t>−</m:t>
+                                    </m:r>
+                                    <m:sSup>
+                                      <m:sSupPr>
+                                        <m:ctrlPr>
+                                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                        </m:ctrlPr>
+                                      </m:sSupPr>
+                                      <m:e>
+                                        <m:sSub>
+                                          <m:sSubPr>
+                                            <m:ctrlPr>
+                                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                            </m:ctrlPr>
+                                          </m:sSubPr>
+                                          <m:e>
+                                            <m:r>
+                                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑟</m:t>
+                                            </m:r>
+                                          </m:e>
+                                          <m:sub>
+                                            <m:r>
+                                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                              </a:rPr>
+                                              <m:t>𝑖𝑗</m:t>
+                                            </m:r>
+                                          </m:sub>
+                                        </m:sSub>
+                                      </m:e>
+                                      <m:sup>
+                                        <m:r>
+                                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                          </a:rPr>
+                                          <m:t>0</m:t>
+                                        </m:r>
+                                      </m:sup>
+                                    </m:sSup>
+                                  </m:e>
+                                </m:d>
+                              </m:sup>
+                            </m:sSup>
+                          </m:e>
+                        </m:d>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                    <m:r>
+                      <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>−1] −</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:sSub>
+                          <m:sSubPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSubPr>
+                          <m:e>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝐵</m:t>
+                            </m:r>
+                          </m:e>
+                          <m:sub>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>𝑖𝑗</m:t>
+                            </m:r>
+                          </m:sub>
+                        </m:sSub>
+                      </m:num>
+                      <m:den>
+                        <m:sSup>
+                          <m:sSupPr>
+                            <m:ctrlPr>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                            </m:ctrlPr>
+                          </m:sSupPr>
+                          <m:e>
+                            <m:sSub>
+                              <m:sSubPr>
+                                <m:ctrlPr>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                </m:ctrlPr>
+                              </m:sSubPr>
+                              <m:e>
+                                <m:r>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑟</m:t>
+                                </m:r>
+                              </m:e>
+                              <m:sub>
+                                <m:r>
+                                  <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                                  </a:rPr>
+                                  <m:t>𝑖𝑗</m:t>
+                                </m:r>
+                              </m:sub>
+                            </m:sSub>
+                          </m:e>
+                          <m:sup>
+                            <m:r>
+                              <a:rPr lang="es-ES" sz="1800" b="0" i="1">
+                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                              </a:rPr>
+                              <m:t>12</m:t>
+                            </m:r>
+                          </m:sup>
+                        </m:sSup>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1800"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA944D43-B7D7-C647-9E99-CF016FFF9D81}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4756150" y="6337300"/>
+              <a:ext cx="4591050" cy="749300"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑞</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑞</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑗</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t> </a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑒</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>^</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>)/</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-ES" sz="1800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟+𝐷_𝑖𝑗 [(1−𝑒^(−𝑎_𝑖𝑗 (𝑟_𝑖𝑗−〖𝑟_𝑖𝑗〗^0 ) ) )^2−1] −𝐵_𝑖𝑗/〖𝑟_𝑖𝑗〗^12 </a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1800"/>
             </a:p>
@@ -1483,15 +2543,15 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="66.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="23.6640625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.1640625" style="9" bestFit="1" customWidth="1"/>
@@ -1529,445 +2589,441 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="39" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="23">
+        <v>2</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="28">
-        <v>2</v>
-      </c>
-      <c r="F2" s="32" t="s">
+      <c r="G2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="H2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="I2" s="21" t="s">
         <v>14</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="25"/>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="31"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="18"/>
       <c r="M3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="32">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="37" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="18.75" customHeight="1">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="38"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="27"/>
       <c r="I5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="31.25" customHeight="1">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="31"/>
-      <c r="G6" s="25"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="19"/>
       <c r="H6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="31.25" customHeight="1">
-      <c r="A7" s="25"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="25"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="32">
-      <c r="A8" s="25"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="25"/>
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="48">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="25"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="21" t="s">
         <v>25</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="32">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="29"/>
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="19"/>
+      <c r="H10" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="24" t="s">
+      <c r="A11" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="28"/>
+      <c r="D11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="23">
+        <v>2</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="28">
-        <v>2</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="H11" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="21" t="s">
         <v>31</v>
-      </c>
-      <c r="I11" s="32" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="31"/>
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="18"/>
     </row>
     <row r="13" spans="1:13" ht="32">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="25"/>
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="I13" s="31"/>
+        <v>32</v>
+      </c>
+      <c r="I13" s="18"/>
     </row>
     <row r="14" spans="1:13" ht="48">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="32" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="18"/>
     </row>
     <row r="15" spans="1:13" ht="48">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="25"/>
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="I15" s="31"/>
+        <v>35</v>
+      </c>
+      <c r="I15" s="18"/>
     </row>
     <row r="16" spans="1:13" ht="64">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="28"/>
+      <c r="D16" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="E16" s="28">
-        <v>2</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" ht="32">
-      <c r="A17" s="25"/>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="29"/>
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="20"/>
       <c r="F17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="19"/>
+      <c r="H17" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="G17" s="25"/>
-      <c r="H17" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" ht="112">
-      <c r="A18" s="25"/>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="29"/>
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="20"/>
       <c r="F18" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="G18" s="25"/>
-      <c r="H18" s="6" t="s">
+      <c r="I18" s="6" t="s">
         <v>42</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="71.25" customHeight="1">
-      <c r="A19" s="24" t="s">
+      <c r="A19" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="24" t="s">
+      <c r="D19" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="23">
+        <v>3</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="28">
-        <v>3</v>
-      </c>
-      <c r="F19" s="7" t="s">
+      <c r="G19" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="G19" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="80">
-      <c r="A20" s="25"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="29"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="20"/>
       <c r="F20" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="25"/>
-      <c r="H20" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="I20" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="45" customHeight="1">
-      <c r="A21" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="29" t="s">
-        <v>60</v>
+      <c r="A21" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>59</v>
       </c>
       <c r="E21" s="8">
         <v>2</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="G21" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="16">
-      <c r="A22" s="25"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="29"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
       <c r="E22" s="8">
         <v>2</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
+        <v>53</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="18"/>
     </row>
     <row r="23" spans="1:9" ht="16">
-      <c r="A23" s="25"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="29"/>
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
       <c r="E23" s="8">
         <v>2</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="G23" s="25"/>
-      <c r="H23" s="31"/>
-      <c r="I23" s="31"/>
+        <v>54</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
     </row>
     <row r="24" spans="1:9" ht="48">
-      <c r="A24" s="25"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="29"/>
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
       <c r="E24" s="8">
         <v>3</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="25"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
+        <v>55</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
     </row>
     <row r="25" spans="1:9" ht="43.25" customHeight="1">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="C25" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="E25" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="20" t="s">
+      <c r="G25" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>69</v>
-      </c>
       <c r="H25" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="48">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="21"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="39"/>
       <c r="F26" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="19"/>
+        <v>65</v>
+      </c>
+      <c r="G26" s="37"/>
       <c r="H26" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1983,34 +3039,8 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="H21:H24"/>
-    <mergeCell ref="I21:I24"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B21:B24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="D21:D24"/>
-    <mergeCell ref="G21:G24"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="D2:D10"/>
-    <mergeCell ref="E2:E10"/>
-    <mergeCell ref="F2:F9"/>
-    <mergeCell ref="G2:G10"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A11:A15"/>
-    <mergeCell ref="B11:B15"/>
-    <mergeCell ref="C11:C15"/>
-    <mergeCell ref="D11:D15"/>
-    <mergeCell ref="E11:E15"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="G11:G15"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I15"/>
-    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="B25:B26"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="G16:G18"/>
     <mergeCell ref="A19:A20"/>
@@ -2027,8 +3057,34 @@
     <mergeCell ref="G25:G26"/>
     <mergeCell ref="E25:E26"/>
     <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="G11:G15"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="A11:A15"/>
+    <mergeCell ref="B11:B15"/>
+    <mergeCell ref="C11:C15"/>
+    <mergeCell ref="D11:D15"/>
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="F2:F9"/>
+    <mergeCell ref="G2:G10"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="D2:D10"/>
+    <mergeCell ref="E2:E10"/>
+    <mergeCell ref="H21:H24"/>
+    <mergeCell ref="I21:I24"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="C21:C24"/>
+    <mergeCell ref="D21:D24"/>
+    <mergeCell ref="G21:G24"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>